<commit_message>
mengumpulakan tugas ke 4
</commit_message>
<xml_diff>
--- a/Tugas3_DataBase/Tugas_3 Muhammad Mirlani.xlsx
+++ b/Tugas3_DataBase/Tugas_3 Muhammad Mirlani.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PEMBELAJARAN\MBKM\DataBase\Tugas3_DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF50F814-1702-45C6-A767-DE8E91BC0BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D37E516-BBE3-4BF0-9F2D-54C2BBC27F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{96DCD083-D29A-496B-9799-3FD385EFBDA7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96DCD083-D29A-496B-9799-3FD385EFBDA7}"/>
   </bookViews>
   <sheets>
     <sheet name="File latihan bersama no 2" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="96">
   <si>
     <t>Latihan Normalisasi Database</t>
   </si>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,9 +402,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,14 +409,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,10 +429,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E7619D-5121-4492-9BF4-B2A23909B1F4}">
-  <dimension ref="B3:P68"/>
+  <dimension ref="B3:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +762,7 @@
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
@@ -779,18 +775,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
@@ -1141,7 +1137,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>1</v>
       </c>
@@ -1173,7 +1169,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>1</v>
       </c>
@@ -1205,7 +1201,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>2</v>
       </c>
@@ -1237,7 +1233,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>2</v>
       </c>
@@ -1269,7 +1265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>3</v>
       </c>
@@ -1301,7 +1297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>4</v>
       </c>
@@ -1333,7 +1329,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>5</v>
       </c>
@@ -1365,7 +1361,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>5</v>
       </c>
@@ -1397,44 +1393,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>53</v>
       </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="C28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="10"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C29" s="1">
         <v>1</v>
       </c>
@@ -1450,14 +1438,11 @@
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C30" s="1">
         <v>2</v>
       </c>
@@ -1473,12 +1458,9 @@
       <c r="G30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C31" s="1">
         <v>3</v>
       </c>
@@ -1494,12 +1476,9 @@
       <c r="G31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H31" s="9"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C32" s="1">
         <v>4</v>
       </c>
@@ -1515,12 +1494,9 @@
       <c r="G32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C33" s="1">
@@ -1538,36 +1514,36 @@
       <c r="G33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C36" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="7" t="s">
+      <c r="C36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H36" s="7" t="s">
+      <c r="H36" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C37" s="1">
@@ -1576,10 +1552,10 @@
       <c r="D37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <v>39448</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="7">
         <v>39452</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -1588,8 +1564,8 @@
       <c r="H37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
@@ -1601,10 +1577,10 @@
       <c r="D38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="7">
         <v>39819</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="7">
         <v>40653</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -1613,8 +1589,8 @@
       <c r="H38" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C39" s="1">
@@ -1623,10 +1599,10 @@
       <c r="D39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <v>40654</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="7">
         <v>42003</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -1635,8 +1611,8 @@
       <c r="H39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C40" s="1">
@@ -1645,10 +1621,10 @@
       <c r="D40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="7">
         <v>40179</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="7">
         <v>40543</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -1657,8 +1633,8 @@
       <c r="H40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C41" s="1">
@@ -1667,10 +1643,10 @@
       <c r="D41" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="7">
         <v>40544</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="7">
         <v>40908</v>
       </c>
       <c r="G41" s="1" t="s">
@@ -1679,8 +1655,8 @@
       <c r="H41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C42" s="1">
@@ -1689,10 +1665,10 @@
       <c r="D42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="7">
         <v>40544</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="7">
         <v>41274</v>
       </c>
       <c r="G42" s="1" t="s">
@@ -1709,10 +1685,10 @@
       <c r="D43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="7">
         <v>40544</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="7">
         <v>41274</v>
       </c>
       <c r="G43" s="1" t="s">
@@ -1729,10 +1705,10 @@
       <c r="D44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="7">
         <v>39814</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="7">
         <v>40543</v>
       </c>
       <c r="G44" s="1" t="s">
@@ -1749,10 +1725,10 @@
       <c r="D45" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="7">
         <v>40179</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="7">
         <v>40908</v>
       </c>
       <c r="G45" s="1" t="s">
@@ -1771,292 +1747,319 @@
       <c r="B49" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E49" s="7" t="s">
+      <c r="C49" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="11" t="s">
         <v>52</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="I49" t="s">
         <v>58</v>
       </c>
-      <c r="J49" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K49" s="13" t="s">
+      <c r="J49" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K49" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L49" s="13" t="s">
+      <c r="L49" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M49" s="13" t="s">
+      <c r="M49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N49" s="13" t="s">
+      <c r="N49" s="11" t="s">
         <v>61</v>
       </c>
       <c r="O49" s="1"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="C50" s="12">
+        <v>1</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J50" s="14">
-        <v>1</v>
-      </c>
-      <c r="K50" s="14" t="s">
+      <c r="G50" s="12">
+        <v>1</v>
+      </c>
+      <c r="J50" s="12">
+        <v>1</v>
+      </c>
+      <c r="K50" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L50" s="17">
+      <c r="L50" s="15">
         <v>39448</v>
       </c>
-      <c r="M50" s="17">
+      <c r="M50" s="15">
         <v>39452</v>
       </c>
-      <c r="N50" s="14">
+      <c r="N50" s="12">
         <v>1</v>
       </c>
       <c r="O50" s="1"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="C51" s="12">
+        <v>1</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J51" s="14">
-        <v>1</v>
-      </c>
-      <c r="K51" s="14" t="s">
+      <c r="G51" s="12">
+        <v>2</v>
+      </c>
+      <c r="J51" s="12">
+        <v>1</v>
+      </c>
+      <c r="K51" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="L51" s="17">
+      <c r="L51" s="15">
         <v>39819</v>
       </c>
-      <c r="M51" s="17">
+      <c r="M51" s="15">
         <v>40653</v>
       </c>
-      <c r="N51" s="14">
+      <c r="N51" s="12">
         <v>3</v>
       </c>
       <c r="O51" s="1"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="C52" s="12">
+        <v>1</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J52" s="14">
-        <v>1</v>
-      </c>
-      <c r="K52" s="14" t="s">
+      <c r="G52" s="12">
+        <v>3</v>
+      </c>
+      <c r="J52" s="12">
+        <v>1</v>
+      </c>
+      <c r="K52" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L52" s="17">
+      <c r="L52" s="15">
         <v>40654</v>
       </c>
-      <c r="M52" s="17">
+      <c r="M52" s="15">
         <v>42003</v>
       </c>
-      <c r="N52" s="14">
+      <c r="N52" s="12">
         <v>4</v>
       </c>
       <c r="O52" s="1"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C53" s="1">
-        <v>2</v>
-      </c>
-      <c r="D53" s="1" t="s">
+      <c r="C53" s="12">
+        <v>2</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J53" s="14">
-        <v>2</v>
-      </c>
-      <c r="K53" s="14" t="s">
+      <c r="G53" s="12">
+        <v>2</v>
+      </c>
+      <c r="J53" s="12">
+        <v>2</v>
+      </c>
+      <c r="K53" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L53" s="17">
+      <c r="L53" s="15">
         <v>40179</v>
       </c>
-      <c r="M53" s="17">
+      <c r="M53" s="15">
         <v>40543</v>
       </c>
-      <c r="N53" s="14">
+      <c r="N53" s="12">
         <v>3</v>
       </c>
       <c r="O53" s="1"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C54" s="1">
-        <v>2</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="C54" s="12">
+        <v>2</v>
+      </c>
+      <c r="D54" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J54" s="14">
-        <v>2</v>
-      </c>
-      <c r="K54" s="14" t="s">
+      <c r="G54" s="12">
+        <v>1</v>
+      </c>
+      <c r="J54" s="12">
+        <v>2</v>
+      </c>
+      <c r="K54" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L54" s="17">
+      <c r="L54" s="15">
         <v>40544</v>
       </c>
-      <c r="M54" s="17">
+      <c r="M54" s="15">
         <v>40908</v>
       </c>
-      <c r="N54" s="14">
+      <c r="N54" s="12">
         <v>4</v>
       </c>
       <c r="O54" s="1"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C55" s="1">
+      <c r="C55" s="12">
         <v>3</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J55" s="14">
+      <c r="G55" s="12">
+        <v>2</v>
+      </c>
+      <c r="J55" s="12">
         <v>3</v>
       </c>
-      <c r="K55" s="14" t="s">
+      <c r="K55" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="L55" s="17">
+      <c r="L55" s="15">
         <v>40544</v>
       </c>
-      <c r="M55" s="17">
+      <c r="M55" s="15">
         <v>41274</v>
       </c>
-      <c r="N55" s="14">
+      <c r="N55" s="12">
         <v>5</v>
       </c>
       <c r="O55" s="1"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C56" s="1">
+      <c r="C56" s="12">
         <v>4</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J56" s="14">
+      <c r="G56" s="12">
+        <v>1</v>
+      </c>
+      <c r="J56" s="12">
         <v>4</v>
       </c>
-      <c r="K56" s="14" t="s">
+      <c r="K56" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="L56" s="17">
+      <c r="L56" s="15">
         <v>40544</v>
       </c>
-      <c r="M56" s="17">
+      <c r="M56" s="15">
         <v>41274</v>
       </c>
-      <c r="N56" s="14">
+      <c r="N56" s="12">
         <v>4</v>
       </c>
       <c r="O56" s="1"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C57" s="1">
+      <c r="C57" s="12">
         <v>5</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="J57" s="14">
+      <c r="G57" s="12">
+        <v>1</v>
+      </c>
+      <c r="J57" s="12">
         <v>5</v>
       </c>
-      <c r="K57" s="14" t="s">
+      <c r="K57" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L57" s="17">
+      <c r="L57" s="15">
         <v>39814</v>
       </c>
-      <c r="M57" s="17">
+      <c r="M57" s="15">
         <v>40543</v>
       </c>
-      <c r="N57" s="14">
+      <c r="N57" s="12">
         <v>6</v>
       </c>
       <c r="O57" s="1"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J58" s="14">
+      <c r="J58" s="12">
         <v>5</v>
       </c>
-      <c r="K58" s="17" t="s">
+      <c r="K58" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="L58" s="17">
+      <c r="L58" s="15">
         <v>40179</v>
       </c>
-      <c r="M58" s="17">
+      <c r="M58" s="15">
         <v>40908</v>
       </c>
-      <c r="N58" s="14">
+      <c r="N58" s="12">
         <v>7</v>
       </c>
       <c r="O58" s="1"/>
@@ -2065,158 +2068,158 @@
       <c r="B60" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D60" s="11" t="s">
         <v>4</v>
       </c>
       <c r="G60" t="s">
         <v>60</v>
       </c>
-      <c r="H60" s="13" t="s">
+      <c r="H60" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I60" s="15" t="s">
+      <c r="I60" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J60" s="16" t="s">
+      <c r="J60" s="14" t="s">
         <v>62</v>
       </c>
       <c r="L60" t="s">
         <v>63</v>
       </c>
-      <c r="M60" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="N60" s="13" t="s">
+      <c r="M60" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N60" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C61" s="14">
-        <v>1</v>
-      </c>
-      <c r="D61" s="14" t="s">
+      <c r="C61" s="12">
+        <v>1</v>
+      </c>
+      <c r="D61" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H61" s="14">
-        <v>1</v>
-      </c>
-      <c r="I61" s="14" t="s">
+      <c r="H61" s="12">
+        <v>1</v>
+      </c>
+      <c r="I61" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J61" s="14">
-        <v>2</v>
-      </c>
-      <c r="M61" s="14">
-        <v>1</v>
-      </c>
-      <c r="N61" s="14" t="s">
+      <c r="J61" s="12">
+        <v>2</v>
+      </c>
+      <c r="M61" s="12">
+        <v>1</v>
+      </c>
+      <c r="N61" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C62" s="14">
-        <v>2</v>
-      </c>
-      <c r="D62" s="14" t="s">
+      <c r="C62" s="12">
+        <v>2</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H62" s="14">
-        <v>2</v>
-      </c>
-      <c r="I62" s="14" t="s">
+      <c r="H62" s="12">
+        <v>2</v>
+      </c>
+      <c r="I62" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J62" s="14">
+      <c r="J62" s="12">
         <v>3</v>
       </c>
-      <c r="M62" s="14">
-        <v>2</v>
-      </c>
-      <c r="N62" s="14" t="s">
+      <c r="M62" s="12">
+        <v>2</v>
+      </c>
+      <c r="N62" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C63" s="14">
+      <c r="C63" s="12">
         <v>3</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H63" s="14">
+      <c r="H63" s="12">
         <v>3</v>
       </c>
-      <c r="I63" s="14" t="s">
+      <c r="I63" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J63" s="14">
-        <v>1</v>
-      </c>
-      <c r="M63" s="14">
+      <c r="J63" s="12">
+        <v>1</v>
+      </c>
+      <c r="M63" s="12">
         <v>3</v>
       </c>
-      <c r="N63" s="14" t="s">
+      <c r="N63" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="H64" s="14">
+      <c r="H64" s="12">
         <v>4</v>
       </c>
-      <c r="I64" s="14" t="s">
+      <c r="I64" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J64" s="14">
-        <v>2</v>
-      </c>
-      <c r="M64" s="14">
+      <c r="J64" s="12">
+        <v>2</v>
+      </c>
+      <c r="M64" s="12">
         <v>4</v>
       </c>
-      <c r="N64" s="14" t="s">
+      <c r="N64" s="12" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="H65" s="14">
+      <c r="H65" s="12">
         <v>5</v>
       </c>
-      <c r="I65" s="14" t="s">
+      <c r="I65" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J65" s="14">
+      <c r="J65" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="66" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="H66" s="14">
+      <c r="H66" s="12">
         <v>6</v>
       </c>
-      <c r="I66" s="14" t="s">
+      <c r="I66" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="J66" s="14">
+      <c r="J66" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="67" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="H67" s="14">
+      <c r="H67" s="12">
         <v>7</v>
       </c>
-      <c r="I67" s="14" t="s">
+      <c r="I67" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="J67" s="14">
+      <c r="J67" s="12">
         <v>3</v>
       </c>
     </row>
@@ -2237,7 +2240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57B7980-3C3F-4DEF-AA24-641E0F9945D4}">
   <dimension ref="B5:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
@@ -2267,253 +2270,253 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12">
         <v>10001</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="15">
         <v>43831</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="15">
         <v>43891</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="14">
-        <v>2</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
+      <c r="B8" s="12">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>3</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>4</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="17">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="15">
         <v>43892</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="15">
         <v>43923</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>5</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="17">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="15">
         <v>44046</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="15">
         <v>44107</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>6</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="17">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="15">
         <v>43955</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="15">
         <v>43955</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>7</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <v>10032</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="15">
         <v>43862</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="15">
         <v>43862</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>8</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="17">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="15">
         <v>43923</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="15">
         <v>44014</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="14">
+      <c r="B15" s="12">
         <v>9</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="17">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="15">
         <v>43954</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="15">
         <v>44107</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="14">
+      <c r="B16" s="12">
         <v>10</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="12">
         <v>10044</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="15">
         <v>43925</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="15">
         <v>43955</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="14">
+      <c r="B17" s="12">
         <v>11</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>10021</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="14">
+      <c r="B18" s="12">
         <v>12</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2523,301 +2526,301 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="14">
-        <v>1</v>
-      </c>
-      <c r="C25" s="14">
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12">
         <v>10001</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="15">
         <v>43831</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="15">
         <v>43891</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="14">
-        <v>2</v>
-      </c>
-      <c r="C26" s="14">
+      <c r="B26" s="12">
+        <v>2</v>
+      </c>
+      <c r="C26" s="12">
         <v>10001</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="14">
+      <c r="B27" s="12">
         <v>3</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="12">
         <v>10001</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="14">
+      <c r="B28" s="12">
         <v>4</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="12">
         <v>10001</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="15">
         <v>43892</v>
       </c>
-      <c r="G28" s="17">
+      <c r="G28" s="15">
         <v>43923</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="14">
+      <c r="B29" s="12">
         <v>5</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="12">
         <v>10001</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="15">
         <v>44046</v>
       </c>
-      <c r="G29" s="17">
+      <c r="G29" s="15">
         <v>44107</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="14">
+      <c r="B30" s="12">
         <v>6</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="12">
         <v>10001</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="15">
         <v>43955</v>
       </c>
-      <c r="G30" s="17">
+      <c r="G30" s="15">
         <v>43955</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="14">
+      <c r="B31" s="12">
         <v>7</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="12">
         <v>10032</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F31" s="15">
         <v>43862</v>
       </c>
-      <c r="G31" s="17">
+      <c r="G31" s="15">
         <v>43862</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="14">
+      <c r="B32" s="12">
         <v>8</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="12">
         <v>10032</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="15">
         <v>43923</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="15">
         <v>44014</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B33" s="14">
+      <c r="B33" s="12">
         <v>9</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="12">
         <v>10032</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F33" s="15">
         <v>43954</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G33" s="15">
         <v>44107</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B34" s="14">
+      <c r="B34" s="12">
         <v>10</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="12">
         <v>10044</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="15">
         <v>43925</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G34" s="15">
         <v>43955</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B35" s="14">
+      <c r="B35" s="12">
         <v>11</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="12">
         <v>10021</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B36" s="14">
+      <c r="B36" s="12">
         <v>12</v>
       </c>
-      <c r="C36" s="14">
+      <c r="C36" s="12">
         <v>10021</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="12" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2827,298 +2830,298 @@
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="H41" s="18" t="s">
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="H41" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="I42" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J42" s="13" t="s">
+      <c r="J42" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="K42" s="13" t="s">
+      <c r="K42" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B43" s="14">
-        <v>1</v>
-      </c>
-      <c r="C43" s="17">
+      <c r="B43" s="12">
+        <v>1</v>
+      </c>
+      <c r="C43" s="15">
         <v>43831</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="15">
         <v>43891</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F43" s="14">
-        <v>1</v>
-      </c>
-      <c r="H43" s="14">
-        <v>1</v>
-      </c>
-      <c r="I43" s="14">
+      <c r="F43" s="12">
+        <v>1</v>
+      </c>
+      <c r="H43" s="12">
+        <v>1</v>
+      </c>
+      <c r="I43" s="12">
         <v>10001</v>
       </c>
-      <c r="J43" s="14" t="s">
+      <c r="J43" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K43" s="14" t="s">
+      <c r="K43" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B44" s="14">
-        <v>2</v>
-      </c>
-      <c r="C44" s="14" t="s">
+      <c r="B44" s="12">
+        <v>2</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F44" s="14">
-        <v>1</v>
-      </c>
-      <c r="H44" s="14">
-        <v>2</v>
-      </c>
-      <c r="I44" s="14">
+      <c r="F44" s="12">
+        <v>1</v>
+      </c>
+      <c r="H44" s="12">
+        <v>2</v>
+      </c>
+      <c r="I44" s="12">
         <v>10032</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="K44" s="14" t="s">
+      <c r="K44" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B45" s="14">
+      <c r="B45" s="12">
         <v>3</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="14">
-        <v>1</v>
-      </c>
-      <c r="H45" s="14">
+      <c r="F45" s="12">
+        <v>1</v>
+      </c>
+      <c r="H45" s="12">
         <v>3</v>
       </c>
-      <c r="I45" s="14">
+      <c r="I45" s="12">
         <v>10044</v>
       </c>
-      <c r="J45" s="14" t="s">
+      <c r="J45" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="K45" s="14" t="s">
+      <c r="K45" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B46" s="14">
+      <c r="B46" s="12">
         <v>4</v>
       </c>
-      <c r="C46" s="17">
+      <c r="C46" s="15">
         <v>43892</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="15">
         <v>43923</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F46" s="14">
-        <v>1</v>
-      </c>
-      <c r="H46" s="14">
+      <c r="F46" s="12">
+        <v>1</v>
+      </c>
+      <c r="H46" s="12">
         <v>4</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I46" s="12">
         <v>10021</v>
       </c>
-      <c r="J46" s="14" t="s">
+      <c r="J46" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K46" s="14" t="s">
+      <c r="K46" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B47" s="14">
+      <c r="B47" s="12">
         <v>5</v>
       </c>
-      <c r="C47" s="17">
+      <c r="C47" s="15">
         <v>44046</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="15">
         <v>44107</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B48" s="14">
+      <c r="B48" s="12">
         <v>6</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="15">
         <v>43955</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="15">
         <v>43955</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F48" s="14">
+      <c r="F48" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B49" s="14">
+      <c r="B49" s="12">
         <v>7</v>
       </c>
-      <c r="C49" s="17">
+      <c r="C49" s="15">
         <v>43862</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="15">
         <v>43862</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B50" s="14">
+      <c r="B50" s="12">
         <v>8</v>
       </c>
-      <c r="C50" s="17">
+      <c r="C50" s="15">
         <v>43923</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="15">
         <v>44014</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F50" s="14">
+      <c r="F50" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B51" s="14">
+      <c r="B51" s="12">
         <v>9</v>
       </c>
-      <c r="C51" s="17">
+      <c r="C51" s="15">
         <v>43954</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="15">
         <v>44107</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F51" s="14">
+      <c r="F51" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B52" s="14">
+      <c r="B52" s="12">
         <v>10</v>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="15">
         <v>43925</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="15">
         <v>43955</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F52" s="14">
+      <c r="F52" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B53" s="14">
+      <c r="B53" s="12">
         <v>11</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F53" s="14">
+      <c r="F53" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B54" s="14">
+      <c r="B54" s="12">
         <v>12</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F54" s="14">
+      <c r="F54" s="12">
         <v>4</v>
       </c>
     </row>
@@ -3128,320 +3131,320 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="I58" s="19" t="s">
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="I58" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="J58" s="19"/>
-      <c r="L58" s="18" t="s">
+      <c r="J58" s="17"/>
+      <c r="L58" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="M58" s="18"/>
-      <c r="N58" s="18"/>
-      <c r="O58" s="18"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F59" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I59" s="13" t="s">
+      <c r="I59" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J59" s="13" t="s">
+      <c r="J59" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="L59" s="13" t="s">
+      <c r="L59" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="M59" s="13" t="s">
+      <c r="M59" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="N59" s="13" t="s">
+      <c r="N59" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="O59" s="13" t="s">
+      <c r="O59" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B60" s="14">
-        <v>1</v>
-      </c>
-      <c r="C60" s="17">
+      <c r="B60" s="12">
+        <v>1</v>
+      </c>
+      <c r="C60" s="15">
         <v>43831</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="15">
         <v>43891</v>
       </c>
-      <c r="E60" s="14">
-        <v>1</v>
-      </c>
-      <c r="F60" s="14">
-        <v>1</v>
-      </c>
-      <c r="I60" s="14">
-        <v>1</v>
-      </c>
-      <c r="J60" s="14" t="s">
+      <c r="E60" s="12">
+        <v>1</v>
+      </c>
+      <c r="F60" s="12">
+        <v>1</v>
+      </c>
+      <c r="I60" s="12">
+        <v>1</v>
+      </c>
+      <c r="J60" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L60" s="14">
-        <v>1</v>
-      </c>
-      <c r="M60" s="14">
+      <c r="L60" s="12">
+        <v>1</v>
+      </c>
+      <c r="M60" s="12">
         <v>10001</v>
       </c>
-      <c r="N60" s="14" t="s">
+      <c r="N60" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="O60" s="14" t="s">
+      <c r="O60" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B61" s="14">
-        <v>2</v>
-      </c>
-      <c r="C61" s="14" t="s">
+      <c r="B61" s="12">
+        <v>2</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E61" s="14">
-        <v>2</v>
-      </c>
-      <c r="F61" s="14">
-        <v>1</v>
-      </c>
-      <c r="I61" s="14">
-        <v>2</v>
-      </c>
-      <c r="J61" s="14" t="s">
+      <c r="E61" s="12">
+        <v>2</v>
+      </c>
+      <c r="F61" s="12">
+        <v>1</v>
+      </c>
+      <c r="I61" s="12">
+        <v>2</v>
+      </c>
+      <c r="J61" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="L61" s="14">
-        <v>2</v>
-      </c>
-      <c r="M61" s="14">
+      <c r="L61" s="12">
+        <v>2</v>
+      </c>
+      <c r="M61" s="12">
         <v>10032</v>
       </c>
-      <c r="N61" s="14" t="s">
+      <c r="N61" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="O61" s="14" t="s">
+      <c r="O61" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B62" s="14">
+      <c r="B62" s="12">
         <v>3</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E62" s="14">
-        <v>2</v>
-      </c>
-      <c r="F62" s="14">
-        <v>1</v>
-      </c>
-      <c r="L62" s="14">
+      <c r="E62" s="12">
+        <v>2</v>
+      </c>
+      <c r="F62" s="12">
+        <v>1</v>
+      </c>
+      <c r="L62" s="12">
         <v>3</v>
       </c>
-      <c r="M62" s="14">
+      <c r="M62" s="12">
         <v>10044</v>
       </c>
-      <c r="N62" s="14" t="s">
+      <c r="N62" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="O62" s="14" t="s">
+      <c r="O62" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B63" s="14">
+      <c r="B63" s="12">
         <v>4</v>
       </c>
-      <c r="C63" s="17">
+      <c r="C63" s="15">
         <v>43892</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D63" s="15">
         <v>43923</v>
       </c>
-      <c r="E63" s="14">
-        <v>1</v>
-      </c>
-      <c r="F63" s="14">
-        <v>1</v>
-      </c>
-      <c r="L63" s="14">
+      <c r="E63" s="12">
+        <v>1</v>
+      </c>
+      <c r="F63" s="12">
+        <v>1</v>
+      </c>
+      <c r="L63" s="12">
         <v>4</v>
       </c>
-      <c r="M63" s="14">
+      <c r="M63" s="12">
         <v>10021</v>
       </c>
-      <c r="N63" s="14" t="s">
+      <c r="N63" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="O63" s="14" t="s">
+      <c r="O63" s="12" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B64" s="14">
+      <c r="B64" s="12">
         <v>5</v>
       </c>
-      <c r="C64" s="17">
+      <c r="C64" s="15">
         <v>44046</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="15">
         <v>44107</v>
       </c>
-      <c r="E64" s="14">
-        <v>1</v>
-      </c>
-      <c r="F64" s="14">
+      <c r="E64" s="12">
+        <v>1</v>
+      </c>
+      <c r="F64" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B65" s="14">
+      <c r="B65" s="12">
         <v>6</v>
       </c>
-      <c r="C65" s="17">
+      <c r="C65" s="15">
         <v>43955</v>
       </c>
-      <c r="D65" s="17">
+      <c r="D65" s="15">
         <v>43955</v>
       </c>
-      <c r="E65" s="14">
-        <v>2</v>
-      </c>
-      <c r="F65" s="14">
+      <c r="E65" s="12">
+        <v>2</v>
+      </c>
+      <c r="F65" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B66" s="14">
+      <c r="B66" s="12">
         <v>7</v>
       </c>
-      <c r="C66" s="17">
+      <c r="C66" s="15">
         <v>43862</v>
       </c>
-      <c r="D66" s="17">
+      <c r="D66" s="15">
         <v>43862</v>
       </c>
-      <c r="E66" s="14">
-        <v>2</v>
-      </c>
-      <c r="F66" s="14">
+      <c r="E66" s="12">
+        <v>2</v>
+      </c>
+      <c r="F66" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B67" s="14">
+      <c r="B67" s="12">
         <v>8</v>
       </c>
-      <c r="C67" s="17">
+      <c r="C67" s="15">
         <v>43923</v>
       </c>
-      <c r="D67" s="17">
+      <c r="D67" s="15">
         <v>44014</v>
       </c>
-      <c r="E67" s="14">
-        <v>2</v>
-      </c>
-      <c r="F67" s="14">
+      <c r="E67" s="12">
+        <v>2</v>
+      </c>
+      <c r="F67" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="14">
+      <c r="B68" s="12">
         <v>9</v>
       </c>
-      <c r="C68" s="17">
+      <c r="C68" s="15">
         <v>43954</v>
       </c>
-      <c r="D68" s="17">
+      <c r="D68" s="15">
         <v>44107</v>
       </c>
-      <c r="E68" s="14">
-        <v>1</v>
-      </c>
-      <c r="F68" s="14">
+      <c r="E68" s="12">
+        <v>1</v>
+      </c>
+      <c r="F68" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B69" s="14">
+      <c r="B69" s="12">
         <v>10</v>
       </c>
-      <c r="C69" s="17">
+      <c r="C69" s="15">
         <v>43925</v>
       </c>
-      <c r="D69" s="17">
+      <c r="D69" s="15">
         <v>43955</v>
       </c>
-      <c r="E69" s="14">
-        <v>2</v>
-      </c>
-      <c r="F69" s="14">
+      <c r="E69" s="12">
+        <v>2</v>
+      </c>
+      <c r="F69" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="14">
+      <c r="B70" s="12">
         <v>11</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E70" s="14">
-        <v>1</v>
-      </c>
-      <c r="F70" s="14">
+      <c r="E70" s="12">
+        <v>1</v>
+      </c>
+      <c r="F70" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B71" s="14">
+      <c r="B71" s="12">
         <v>12</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D71" s="14" t="s">
+      <c r="D71" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E71" s="14">
-        <v>2</v>
-      </c>
-      <c r="F71" s="14">
+      <c r="E71" s="12">
+        <v>2</v>
+      </c>
+      <c r="F71" s="12">
         <v>4</v>
       </c>
     </row>

</xml_diff>